<commit_message>
Removing description and fixing sequencer test.
</commit_message>
<xml_diff>
--- a/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
+++ b/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassonmx\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Tools\ExpensifyImporter\src\ExpensifyImporter\Tests\ExpensifyImporter.UnitTests\Modules\Sequencing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCFB098-3F7D-4629-84A6-A70E65698D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B4DCD7-AA3E-43C5-99C2-4C01AD5B29D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="31910" windowHeight="18430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expensify Report Export" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Timestamp</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Category</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>Receipt</t>
@@ -459,19 +456,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" customWidth="1"/>
-    <col min="2" max="6" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" customWidth="1"/>
+    <col min="2" max="5" width="11.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,175 +484,172 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>6.67</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>28.25</v>
       </c>
       <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>28.25</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
       <c r="C5">
         <v>6.43</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>6.43</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
       <c r="C7">
         <v>4.99</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>6.43</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
       <c r="C9">
         <v>16.350000000000001</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>6.43</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{EB67F85C-3066-4E76-9787-7EB11A40E4CA}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{EB67F85C-3066-4E76-9787-7EB11A40E4CA}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
update to get covering tests working for excelToDatabase sequencer.
</commit_message>
<xml_diff>
--- a/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
+++ b/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Tools\ExpensifyImporter\src\ExpensifyImporter\Tests\ExpensifyImporter.UnitTests\Modules\Sequencing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B4DCD7-AA3E-43C5-99C2-4C01AD5B29D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AED1144-6DEF-4670-962B-FC696A2F60E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -595,7 +595,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>6.43</v>
+        <v>6.44</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -612,7 +612,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>16.350000000000001</v>
+        <v>16.36</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -641,15 +641,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
+    <hyperlink ref="E10" r:id="rId1" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{EB67F85C-3066-4E76-9787-7EB11A40E4CA}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
+    <hyperlink ref="E5" r:id="rId6" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
+    <hyperlink ref="E2" r:id="rId9" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Adding receipt Id and updating tests.
</commit_message>
<xml_diff>
--- a/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
+++ b/src/ExpensifyImporter/Tests/ExpensifyImporter.UnitTests/Modules/Sequencing/Data/Expense_Batch_Test_2017_02_01_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Tools\ExpensifyImporter\src\ExpensifyImporter\Tests\ExpensifyImporter.UnitTests\Modules\Sequencing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AED1144-6DEF-4670-962B-FC696A2F60E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE090ABE-8205-4962-8D5F-48C7BF47C897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="6800" windowWidth="19750" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expensify Report Export" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Timestamp</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>https://www.expensify.com/receipts/w_a445fd27951f1d516f0b67daa93885b95e755e7xxxx9.jpg</t>
+  </si>
+  <si>
+    <t>Receipt Id</t>
   </si>
 </sst>
 </file>
@@ -456,200 +459,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-    <col min="2" max="5" width="11.53125" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" customWidth="1"/>
+    <col min="3" max="6" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>6.67</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>28.25</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>28.25</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>6.43</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>6.43</v>
       </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>4.99</v>
       </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>6.44</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>16.36</v>
       </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>6.43</v>
       </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
-    <hyperlink ref="E8" r:id="rId3" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{EB67F85C-3066-4E76-9787-7EB11A40E4CA}"/>
-    <hyperlink ref="E5" r:id="rId6" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
-    <hyperlink ref="E3" r:id="rId7" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
-    <hyperlink ref="E4" r:id="rId8" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
-    <hyperlink ref="E2" r:id="rId9" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{B9696149-5DAC-4A7E-8DF3-87FC144DAD74}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{170E4357-0BA8-4050-AACA-BFBC6C279ECD}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{8FA1A08D-7DCA-4D83-B457-DE460FA6ADC9}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{ADDA62DA-1927-41D2-B10D-C071711AEC4E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{EB67F85C-3066-4E76-9787-7EB11A40E4CA}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{9343A356-8EB5-49F4-B058-53E01B252083}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{C331B716-81C6-4DD3-B7A8-6EF81A7D2371}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{1F75E045-2DE1-4B97-AF14-D03EB602569E}"/>
+    <hyperlink ref="F2" r:id="rId9" xr:uid="{C5D6D77D-40BB-4BF9-A454-B1040CF95559}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait"/>

</xml_diff>